<commit_message>
Alt2 uses the . notation. I need to know more
</commit_message>
<xml_diff>
--- a/CH-187 Custom Grouping.xlsx
+++ b/CH-187 Custom Grouping.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC79851-5DF0-4ECD-BBD4-A3AE399EE392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1894838B-A1F4-48A1-9B99-3DC012AA0015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="Alt1" sheetId="2" r:id="rId2"/>
+    <sheet name="Alt2" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Alt1'!$A$1:$C$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt2'!$A$1:$C$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$A$1:$C$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -42,8 +44,9 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
+  <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -54,16 +57,30 @@
       </extLst>
     </bk>
   </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="8">
   <si>
     <t>Question</t>
   </si>
@@ -288,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -361,6 +378,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -621,6 +641,66 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>2</v>
+    <v>1</v>
+    <v>32</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="iftab" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -894,7 +974,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="525" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="822" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1235,8 +1315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{897FAE66-81DC-4DB7-A9BB-5CEA723EEECB}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.5"/>
@@ -1693,4 +1773,332 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5154BEB6-3B73-4276-9637-D63F30838496}">
+  <dimension ref="A1:L23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="6.77734375" customWidth="1"/>
+    <col min="2" max="2" width="11" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="6" width="4.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11" style="5" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="E1"/>
+      <c r="G1" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="27"/>
+      <c r="K1" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2"/>
+      <c r="G2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B3" s="18">
+        <v>45292</v>
+      </c>
+      <c r="C3" s="19">
+        <v>26</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3"/>
+      <c r="G3" s="12">
+        <v>1</v>
+      </c>
+      <c r="H3" s="13">
+        <v>137</v>
+      </c>
+      <c r="I3" s="10"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B4" s="18">
+        <v>45293</v>
+      </c>
+      <c r="C4" s="19">
+        <v>19</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4"/>
+      <c r="G4" s="12">
+        <v>2</v>
+      </c>
+      <c r="H4" s="13">
+        <v>27</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B5" s="18">
+        <v>45293</v>
+      </c>
+      <c r="C5" s="19">
+        <v>10</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5"/>
+      <c r="G5" s="12">
+        <v>3</v>
+      </c>
+      <c r="H5" s="13">
+        <v>140</v>
+      </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="18">
+        <v>45294</v>
+      </c>
+      <c r="C6" s="19">
+        <v>30</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6"/>
+      <c r="G6" s="12">
+        <v>4</v>
+      </c>
+      <c r="H6" s="13">
+        <v>53</v>
+      </c>
+      <c r="I6" s="10"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B7" s="18">
+        <v>45294</v>
+      </c>
+      <c r="C7" s="19">
+        <v>27</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7"/>
+      <c r="G7" s="12">
+        <v>5</v>
+      </c>
+      <c r="H7" s="13">
+        <v>23</v>
+      </c>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B8" s="18">
+        <v>45294</v>
+      </c>
+      <c r="C8" s="19">
+        <v>25</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8"/>
+      <c r="G8" s="5"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+    </row>
+    <row r="9" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="11">
+        <v>45297</v>
+      </c>
+      <c r="C9" s="17">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9"/>
+      <c r="G9" s="5"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+    </row>
+    <row r="10" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B10" s="11">
+        <v>45297</v>
+      </c>
+      <c r="C10" s="17">
+        <v>26</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10"/>
+      <c r="G10" s="5"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+    </row>
+    <row r="11" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="20">
+        <v>45299</v>
+      </c>
+      <c r="C11" s="21">
+        <v>29</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11"/>
+      <c r="G11" s="5"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+    </row>
+    <row r="12" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="20">
+        <v>45299</v>
+      </c>
+      <c r="C12" s="21">
+        <v>24</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12"/>
+      <c r="G12" s="5"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A13" s="2"/>
+      <c r="B13" s="20">
+        <v>45300</v>
+      </c>
+      <c r="C13" s="21">
+        <v>17</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A14" s="2"/>
+      <c r="B14" s="20">
+        <v>45301</v>
+      </c>
+      <c r="C14" s="21">
+        <v>19</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A15" s="2"/>
+      <c r="B15" s="20">
+        <v>45301</v>
+      </c>
+      <c r="C15" s="21">
+        <v>25</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A16" s="2"/>
+      <c r="B16" s="20">
+        <v>45302</v>
+      </c>
+      <c r="C16" s="21">
+        <v>26</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A17" s="2"/>
+      <c r="B17" s="11">
+        <v>45307</v>
+      </c>
+      <c r="C17" s="17">
+        <v>24</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="1"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A18" s="2"/>
+      <c r="B18" s="11">
+        <v>45308</v>
+      </c>
+      <c r="C18" s="17">
+        <v>29</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="B19" s="22">
+        <v>45310</v>
+      </c>
+      <c r="C19" s="23">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="B21" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="234" x14ac:dyDescent="0.5">
+      <c r="B23" s="29" t="e" cm="1" vm="1">
+        <f t="array" ref="B23">_xlfn.LET(
+    _xlpm.d, N(+_xlfn._TRO_TRAILING(B:B)),
+    _xlpm.g, _xlfn.GROUPBY(
+        _xlfn.SCAN(0, _xlfn.DROP(_xlpm.d, 1) - _xlfn.DROP(_xlpm.d, -1) &gt; 1, _xleta.SUM),
+        N(+_xlfn.DROP(_xlfn._TRO_TRAILING(C:C), 1)),
+        _xleta.SUM,
+        ,
+        0
+    ),
+    IF(_xlpm.g, _xlpm.g, {"Group","TotalSales"})
+)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
. notation is called a TRIM reference
</commit_message>
<xml_diff>
--- a/CH-187 Custom Grouping.xlsx
+++ b/CH-187 Custom Grouping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1894838B-A1F4-48A1-9B99-3DC012AA0015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1E3ACD-6501-42BB-B6B1-7608D0ACB09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,9 +44,8 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="2">
+  <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -57,30 +56,16 @@
       </extLst>
     </bk>
   </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="1">
-    <bk>
-      <rc t="2" v="0"/>
-    </bk>
-  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="9">
   <si>
     <t>Question</t>
   </si>
@@ -104,6 +89,9 @@
   </si>
   <si>
     <t>Interesting use of groupby</t>
+  </si>
+  <si>
+    <t>The first use of trim references I have seen.</t>
   </si>
 </sst>
 </file>
@@ -641,66 +629,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <global>
-    <keyFlags>
-      <key name="_Self">
-        <flag name="ExcludeFromFile" value="1"/>
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_DisplayString">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Flags">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Format">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_SubLabel">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Attribution">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Icon">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Display">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_CanonicalPropertyNames">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_ClassificationId">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-    </keyFlags>
-  </global>
-</rvTypesInfo>
-</file>
-
-<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <rv s="0">
-    <v>2</v>
-    <v>1</v>
-    <v>32</v>
-  </rv>
-</rvData>
-</file>
-
-<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <s t="_error">
-    <k n="errorType" t="i"/>
-    <k n="iftab" t="i"/>
-    <k n="subType" t="i"/>
-  </s>
-</rvStructures>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1777,10 +1705,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5154BEB6-3B73-4276-9637-D63F30838496}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.5"/>
@@ -1788,7 +1716,9 @@
     <col min="1" max="1" width="6.77734375" customWidth="1"/>
     <col min="2" max="2" width="11" style="4" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="6" width="4.6640625" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" customWidth="1"/>
     <col min="7" max="7" width="11" style="5" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
@@ -1898,6 +1828,10 @@
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
       <c r="K6" s="7"/>
+      <c r="L6" s="2">
+        <f>N(_xlfn.TRIMRANGE(B:B))</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B7" s="18">
@@ -2073,13 +2007,13 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="B21" s="28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="234" x14ac:dyDescent="0.5">
-      <c r="B23" s="29" t="e" cm="1" vm="1">
-        <f t="array" ref="B23">_xlfn.LET(
+      <c r="E21" s="28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="D23" s="29" t="str" cm="1">
+        <f t="array" ref="D23:E28">_xlfn.LET(
     _xlpm.d, N(+_xlfn._TRO_TRAILING(B:B)),
     _xlpm.g, _xlfn.GROUPBY(
         _xlfn.SCAN(0, _xlfn.DROP(_xlpm.d, 1) - _xlfn.DROP(_xlpm.d, -1) &gt; 1, _xleta.SUM),
@@ -2090,7 +2024,149 @@
     ),
     IF(_xlpm.g, _xlpm.g, {"Group","TotalSales"})
 )</f>
-        <v>#VALUE!</v>
+        <v>Group</v>
+      </c>
+      <c r="E23" t="str">
+        <v>TotalSales</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="H30" s="18" cm="1">
+        <f t="array" ref="H30:H48">_xlfn.LET(
+    _xlpm.d, N(+_xlfn._TRO_TRAILING(B:B)),
+_xlpm.d
+)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="H31" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="H32" s="18">
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H33" s="18">
+        <v>45293</v>
+      </c>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H34" s="18">
+        <v>45293</v>
+      </c>
+    </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H35" s="18">
+        <v>45294</v>
+      </c>
+    </row>
+    <row r="36" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H36" s="11">
+        <v>45294</v>
+      </c>
+    </row>
+    <row r="37" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H37" s="11">
+        <v>45294</v>
+      </c>
+    </row>
+    <row r="38" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H38" s="20">
+        <v>45297</v>
+      </c>
+    </row>
+    <row r="39" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H39" s="20">
+        <v>45297</v>
+      </c>
+    </row>
+    <row r="40" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H40" s="20">
+        <v>45299</v>
+      </c>
+    </row>
+    <row r="41" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H41" s="20">
+        <v>45299</v>
+      </c>
+    </row>
+    <row r="42" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H42" s="20">
+        <v>45300</v>
+      </c>
+    </row>
+    <row r="43" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H43" s="20">
+        <v>45301</v>
+      </c>
+    </row>
+    <row r="44" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H44" s="11">
+        <v>45301</v>
+      </c>
+    </row>
+    <row r="45" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H45" s="11">
+        <v>45302</v>
+      </c>
+    </row>
+    <row r="46" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H46" s="22">
+        <v>45307</v>
+      </c>
+    </row>
+    <row r="47" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H47" s="11">
+        <v>45308</v>
+      </c>
+    </row>
+    <row r="48" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H48" s="22">
+        <v>45310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>